<commit_message>
Student Book a class General
</commit_message>
<xml_diff>
--- a/TestDataXls/375_students.xlsx
+++ b/TestDataXls/375_students.xlsx
@@ -8,16 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test\TestDataXls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48A7613-CB83-4002-A207-F54D211A2AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F80D40-2F85-4EAD-A2CA-3FFC7E4E2F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="profile" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -6723,8 +6732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="B203" sqref="B203"/>
+    <sheetView tabSelected="1" topLeftCell="E319" workbookViewId="0">
+      <selection activeCell="O345" sqref="O345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>